<commit_message>
update 3.5 3.8 3.15 3.18
</commit_message>
<xml_diff>
--- a/刘珊珊/规划/3.8 e享课堂项目预算.xlsx
+++ b/刘珊珊/规划/3.8 e享课堂项目预算.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EFA00D-C5F2-477F-A037-BE7DEF26E391}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200"/>
+    <workbookView xWindow="9870" yWindow="0" windowWidth="7740" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>e享课堂项目预算</t>
   </si>
@@ -220,22 +221,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>￥8000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>￥5000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>￥5000</t>
+    <t>￥13000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -590,11 +583,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -827,7 +820,7 @@
         <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -847,7 +840,7 @@
         <v>39</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>